<commit_message>
Adding entity PurchaseOrderBreakdown and PurchaseInvoice
</commit_message>
<xml_diff>
--- a/documents/Schema_Sheet.xlsx
+++ b/documents/Schema_Sheet.xlsx
@@ -44,9 +44,6 @@
     <t>created_by</t>
   </si>
   <si>
-    <t>Purchase_Order_Detail</t>
-  </si>
-  <si>
     <t>purchase_order_id</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>remarks</t>
+  </si>
+  <si>
+    <t>Purchase_Order_Breakdown</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="B2:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -507,7 +507,7 @@
     <col min="2" max="2" width="14.3046875" customWidth="1"/>
     <col min="3" max="3" width="8.3046875" customWidth="1"/>
     <col min="4" max="4" width="11.15234375" customWidth="1"/>
-    <col min="5" max="5" width="20.23046875" customWidth="1"/>
+    <col min="5" max="5" width="24.921875" customWidth="1"/>
     <col min="6" max="6" width="9.23046875" customWidth="1"/>
     <col min="7" max="8" width="18.3046875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11.765625" bestFit="1" customWidth="1"/>
@@ -519,10 +519,10 @@
       </c>
       <c r="C2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.4">
@@ -534,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.4">
@@ -543,7 +543,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>2</v>
@@ -551,75 +551,75 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.4">
@@ -628,7 +628,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.4">
@@ -637,7 +637,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.4">
@@ -652,65 +652,65 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
       <c r="E18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2"/>
       <c r="E19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B21" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.4">
@@ -719,37 +719,37 @@
       </c>
       <c r="C22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>5</v>
@@ -757,13 +757,13 @@
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>4</v>
@@ -775,7 +775,7 @@
       </c>
       <c r="C26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.4">
@@ -784,17 +784,17 @@
       </c>
       <c r="C27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.4">
       <c r="G28" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.4">
       <c r="G29" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.4">

</xml_diff>